<commit_message>
added bilingual headers test
</commit_message>
<xml_diff>
--- a/src/test/java/data/TestData.xlsx
+++ b/src/test/java/data/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harshal\IdeaProjects\Al_Mulla_exchange\src\test\java\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8937A453-AF55-48D8-9969-C1F8429F6370}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85987B9-57F1-4891-A0AB-54C9FDA78A4E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7425" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -510,7 +510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -574,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C77C054-7946-4AEB-991A-B2F4916E7909}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>